<commit_message>
Update sectoral carbon budgets
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_SRV_UC.xlsx
+++ b/SuppXLS/Scen_B_SRV_UC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\agaur\Documents\Veda\times-ireland-model-sectoral_cb\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF6208E6-537A-4E3D-9BC1-FEDC92C9DD2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2025B393-C336-4090-8463-19E7DA168962}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="17280" windowHeight="8955" xr2:uid="{24C11528-D002-463A-994E-9F1C7B8997EB}"/>
+    <workbookView xWindow="1425" yWindow="4665" windowWidth="18000" windowHeight="12735" xr2:uid="{24C11528-D002-463A-994E-9F1C7B8997EB}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="37" r:id="rId1"/>

</xml_diff>